<commit_message>
DossierInscription, Fiche etudiant, Espace secretaire, gestionnaire,professeur
</commit_message>
<xml_diff>
--- a/Documentations/Gant-JAVA-LPRS.xlsx
+++ b/Documentations/Gant-JAVA-LPRS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krimi\Desktop\Info\ProjetLprs_Java\Documentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetLprs_Java\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7089FF7-54EA-4D9C-A025-CE550CEDA0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36275882-3060-423B-9B68-BFD54E1EA611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0F548F66-3344-4CBB-911B-2A81E54675D2}"/>
   </bookViews>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57744C3F-6280-4959-BECA-99D079BDAE28}">
   <dimension ref="A1:CA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Gestion de stock, vue et OnClick
</commit_message>
<xml_diff>
--- a/Documentations/Gant-JAVA-LPRS.xlsx
+++ b/Documentations/Gant-JAVA-LPRS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetLprs_Java\Documentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Abdallah_Sherazad\ProjetLprs_Java\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B423C4C-F8A6-4D43-92E2-664A3A13191B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025F5E01-8997-4C94-A551-82A2377E3818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0F548F66-3344-4CBB-911B-2A81E54675D2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="33">
   <si>
     <t>Site Lprs</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Krishmini</t>
+  </si>
+  <si>
+    <t>Sherazad</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -515,6 +518,21 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -523,22 +541,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -879,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57744C3F-6280-4959-BECA-99D079BDAE28}">
   <dimension ref="A1:CA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="38" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,186 +1050,186 @@
       <c r="B3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="42">
         <v>45663</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="37">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="42">
         <v>45670</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="37">
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="42">
         <v>45677</v>
       </c>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="37">
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="42">
         <v>45684</v>
       </c>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="38"/>
-      <c r="AD3" s="39"/>
-      <c r="AE3" s="37">
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43"/>
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="42">
         <v>45691</v>
       </c>
-      <c r="AF3" s="38"/>
-      <c r="AG3" s="38"/>
-      <c r="AH3" s="38"/>
-      <c r="AI3" s="38"/>
-      <c r="AJ3" s="38"/>
-      <c r="AK3" s="39"/>
-      <c r="AL3" s="37">
+      <c r="AF3" s="43"/>
+      <c r="AG3" s="43"/>
+      <c r="AH3" s="43"/>
+      <c r="AI3" s="43"/>
+      <c r="AJ3" s="43"/>
+      <c r="AK3" s="44"/>
+      <c r="AL3" s="42">
         <v>45698</v>
       </c>
-      <c r="AM3" s="38"/>
-      <c r="AN3" s="38"/>
-      <c r="AO3" s="38"/>
-      <c r="AP3" s="38"/>
-      <c r="AQ3" s="38"/>
-      <c r="AR3" s="39"/>
-      <c r="AS3" s="37">
+      <c r="AM3" s="43"/>
+      <c r="AN3" s="43"/>
+      <c r="AO3" s="43"/>
+      <c r="AP3" s="43"/>
+      <c r="AQ3" s="43"/>
+      <c r="AR3" s="44"/>
+      <c r="AS3" s="42">
         <v>45705</v>
       </c>
-      <c r="AT3" s="38"/>
-      <c r="AU3" s="38"/>
-      <c r="AV3" s="38"/>
-      <c r="AW3" s="38"/>
-      <c r="AX3" s="38"/>
-      <c r="AY3" s="39"/>
-      <c r="AZ3" s="37">
+      <c r="AT3" s="43"/>
+      <c r="AU3" s="43"/>
+      <c r="AV3" s="43"/>
+      <c r="AW3" s="43"/>
+      <c r="AX3" s="43"/>
+      <c r="AY3" s="44"/>
+      <c r="AZ3" s="42">
         <v>45712</v>
       </c>
-      <c r="BA3" s="38"/>
-      <c r="BB3" s="38"/>
-      <c r="BC3" s="38"/>
-      <c r="BD3" s="38"/>
-      <c r="BE3" s="38"/>
-      <c r="BF3" s="39"/>
-      <c r="BG3" s="37">
+      <c r="BA3" s="43"/>
+      <c r="BB3" s="43"/>
+      <c r="BC3" s="43"/>
+      <c r="BD3" s="43"/>
+      <c r="BE3" s="43"/>
+      <c r="BF3" s="44"/>
+      <c r="BG3" s="42">
         <v>45719</v>
       </c>
-      <c r="BH3" s="38"/>
-      <c r="BI3" s="38"/>
-      <c r="BJ3" s="38"/>
-      <c r="BK3" s="38"/>
-      <c r="BL3" s="38"/>
-      <c r="BM3" s="39"/>
-      <c r="BN3" s="37">
+      <c r="BH3" s="43"/>
+      <c r="BI3" s="43"/>
+      <c r="BJ3" s="43"/>
+      <c r="BK3" s="43"/>
+      <c r="BL3" s="43"/>
+      <c r="BM3" s="44"/>
+      <c r="BN3" s="42">
         <v>45726</v>
       </c>
-      <c r="BO3" s="38"/>
-      <c r="BP3" s="38"/>
-      <c r="BQ3" s="38"/>
-      <c r="BR3" s="38"/>
-      <c r="BS3" s="38"/>
-      <c r="BT3" s="39"/>
-      <c r="BU3" s="37">
+      <c r="BO3" s="43"/>
+      <c r="BP3" s="43"/>
+      <c r="BQ3" s="43"/>
+      <c r="BR3" s="43"/>
+      <c r="BS3" s="43"/>
+      <c r="BT3" s="44"/>
+      <c r="BU3" s="42">
         <v>45726</v>
       </c>
-      <c r="BV3" s="38"/>
-      <c r="BW3" s="38"/>
-      <c r="BX3" s="38"/>
-      <c r="BY3" s="38"/>
-      <c r="BZ3" s="38"/>
-      <c r="CA3" s="39"/>
+      <c r="BV3" s="43"/>
+      <c r="BW3" s="43"/>
+      <c r="BX3" s="43"/>
+      <c r="BY3" s="43"/>
+      <c r="BZ3" s="43"/>
+      <c r="CA3" s="44"/>
     </row>
     <row r="4" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="39"/>
-      <c r="AE4" s="38"/>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="38"/>
-      <c r="AI4" s="38"/>
-      <c r="AJ4" s="38"/>
-      <c r="AK4" s="39"/>
-      <c r="AL4" s="38"/>
-      <c r="AM4" s="38"/>
-      <c r="AN4" s="38"/>
-      <c r="AO4" s="38"/>
-      <c r="AP4" s="38"/>
-      <c r="AQ4" s="38"/>
-      <c r="AR4" s="39"/>
-      <c r="AS4" s="38"/>
-      <c r="AT4" s="38"/>
-      <c r="AU4" s="38"/>
-      <c r="AV4" s="38"/>
-      <c r="AW4" s="38"/>
-      <c r="AX4" s="38"/>
-      <c r="AY4" s="39"/>
-      <c r="AZ4" s="38"/>
-      <c r="BA4" s="38"/>
-      <c r="BB4" s="38"/>
-      <c r="BC4" s="38"/>
-      <c r="BD4" s="38"/>
-      <c r="BE4" s="38"/>
-      <c r="BF4" s="39"/>
-      <c r="BG4" s="38"/>
-      <c r="BH4" s="38"/>
-      <c r="BI4" s="38"/>
-      <c r="BJ4" s="38"/>
-      <c r="BK4" s="38"/>
-      <c r="BL4" s="38"/>
-      <c r="BM4" s="39"/>
-      <c r="BN4" s="38"/>
-      <c r="BO4" s="38"/>
-      <c r="BP4" s="38"/>
-      <c r="BQ4" s="38"/>
-      <c r="BR4" s="38"/>
-      <c r="BS4" s="38"/>
-      <c r="BT4" s="39"/>
-      <c r="BU4" s="38"/>
-      <c r="BV4" s="38"/>
-      <c r="BW4" s="38"/>
-      <c r="BX4" s="38"/>
-      <c r="BY4" s="38"/>
-      <c r="BZ4" s="38"/>
-      <c r="CA4" s="39"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
+      <c r="AG4" s="43"/>
+      <c r="AH4" s="43"/>
+      <c r="AI4" s="43"/>
+      <c r="AJ4" s="43"/>
+      <c r="AK4" s="44"/>
+      <c r="AL4" s="43"/>
+      <c r="AM4" s="43"/>
+      <c r="AN4" s="43"/>
+      <c r="AO4" s="43"/>
+      <c r="AP4" s="43"/>
+      <c r="AQ4" s="43"/>
+      <c r="AR4" s="44"/>
+      <c r="AS4" s="43"/>
+      <c r="AT4" s="43"/>
+      <c r="AU4" s="43"/>
+      <c r="AV4" s="43"/>
+      <c r="AW4" s="43"/>
+      <c r="AX4" s="43"/>
+      <c r="AY4" s="44"/>
+      <c r="AZ4" s="43"/>
+      <c r="BA4" s="43"/>
+      <c r="BB4" s="43"/>
+      <c r="BC4" s="43"/>
+      <c r="BD4" s="43"/>
+      <c r="BE4" s="43"/>
+      <c r="BF4" s="44"/>
+      <c r="BG4" s="43"/>
+      <c r="BH4" s="43"/>
+      <c r="BI4" s="43"/>
+      <c r="BJ4" s="43"/>
+      <c r="BK4" s="43"/>
+      <c r="BL4" s="43"/>
+      <c r="BM4" s="44"/>
+      <c r="BN4" s="43"/>
+      <c r="BO4" s="43"/>
+      <c r="BP4" s="43"/>
+      <c r="BQ4" s="43"/>
+      <c r="BR4" s="43"/>
+      <c r="BS4" s="43"/>
+      <c r="BT4" s="44"/>
+      <c r="BU4" s="43"/>
+      <c r="BV4" s="43"/>
+      <c r="BW4" s="43"/>
+      <c r="BX4" s="43"/>
+      <c r="BY4" s="43"/>
+      <c r="BZ4" s="43"/>
+      <c r="CA4" s="44"/>
     </row>
     <row r="5" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -2376,7 +2378,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="32"/>
@@ -2413,13 +2415,13 @@
       <c r="AI15" s="32"/>
       <c r="AJ15" s="18"/>
       <c r="AK15" s="18"/>
-      <c r="AL15" s="44"/>
-      <c r="AM15" s="44"/>
-      <c r="AN15" s="44"/>
-      <c r="AO15" s="44"/>
-      <c r="AP15" s="44"/>
-      <c r="AQ15" s="45"/>
-      <c r="AR15" s="45"/>
+      <c r="AL15" s="40"/>
+      <c r="AM15" s="40"/>
+      <c r="AN15" s="40"/>
+      <c r="AO15" s="40"/>
+      <c r="AP15" s="40"/>
+      <c r="AQ15" s="41"/>
+      <c r="AR15" s="41"/>
       <c r="AS15" s="32"/>
       <c r="AT15" s="32"/>
       <c r="AU15" s="32"/>
@@ -2880,7 +2882,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="32"/>
@@ -2917,13 +2919,13 @@
       <c r="AI21" s="32"/>
       <c r="AJ21" s="18"/>
       <c r="AK21" s="18"/>
-      <c r="AL21" s="44"/>
-      <c r="AM21" s="44"/>
-      <c r="AN21" s="44"/>
-      <c r="AO21" s="44"/>
-      <c r="AP21" s="44"/>
-      <c r="AQ21" s="45"/>
-      <c r="AR21" s="45"/>
+      <c r="AL21" s="40"/>
+      <c r="AM21" s="40"/>
+      <c r="AN21" s="40"/>
+      <c r="AO21" s="40"/>
+      <c r="AP21" s="40"/>
+      <c r="AQ21" s="41"/>
+      <c r="AR21" s="41"/>
       <c r="AS21" s="32"/>
       <c r="AT21" s="32"/>
       <c r="AU21" s="32"/>
@@ -2960,175 +2962,175 @@
       <c r="BZ21" s="18"/>
       <c r="CA21" s="18"/>
     </row>
-    <row r="22" spans="1:79" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
+    <row r="22" spans="1:79" x14ac:dyDescent="0.3">
+      <c r="A22" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="42"/>
-      <c r="T22" s="42"/>
-      <c r="U22" s="42"/>
-      <c r="V22" s="42"/>
-      <c r="W22" s="41"/>
-      <c r="X22" s="41"/>
-      <c r="Y22" s="42"/>
-      <c r="Z22" s="42"/>
-      <c r="AA22" s="42"/>
-      <c r="AB22" s="42"/>
-      <c r="AC22" s="42"/>
-      <c r="AD22" s="41"/>
-      <c r="AE22" s="42"/>
-      <c r="AF22" s="42"/>
-      <c r="AG22" s="42"/>
-      <c r="AH22" s="42"/>
-      <c r="AI22" s="42"/>
-      <c r="AJ22" s="41"/>
-      <c r="AK22" s="41"/>
-      <c r="AL22" s="44"/>
-      <c r="AM22" s="44"/>
-      <c r="AN22" s="44"/>
-      <c r="AO22" s="44"/>
-      <c r="AP22" s="44"/>
-      <c r="AQ22" s="45"/>
-      <c r="AR22" s="45"/>
-      <c r="AS22" s="42"/>
-      <c r="AT22" s="42"/>
-      <c r="AU22" s="42"/>
-      <c r="AV22" s="42"/>
-      <c r="AW22" s="42"/>
-      <c r="AX22" s="41"/>
-      <c r="AY22" s="41"/>
-      <c r="AZ22" s="42"/>
-      <c r="BA22" s="42"/>
-      <c r="BB22" s="42"/>
-      <c r="BC22" s="42"/>
-      <c r="BD22" s="42"/>
-      <c r="BE22" s="41"/>
-      <c r="BF22" s="41"/>
-      <c r="BG22" s="42"/>
-      <c r="BH22" s="42"/>
-      <c r="BI22" s="42"/>
-      <c r="BJ22" s="42"/>
-      <c r="BK22" s="42"/>
-      <c r="BL22" s="41"/>
-      <c r="BM22" s="41"/>
-      <c r="BN22" s="42"/>
-      <c r="BO22" s="42"/>
-      <c r="BP22" s="42"/>
-      <c r="BQ22" s="42"/>
-      <c r="BR22" s="42"/>
-      <c r="BS22" s="41"/>
-      <c r="BT22" s="41"/>
-      <c r="BU22" s="42"/>
-      <c r="BV22" s="42"/>
-      <c r="BW22" s="42"/>
-      <c r="BX22" s="42"/>
-      <c r="BY22" s="42"/>
-      <c r="BZ22" s="41"/>
-      <c r="CA22" s="41"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="39"/>
+      <c r="S22" s="39"/>
+      <c r="T22" s="39"/>
+      <c r="U22" s="39"/>
+      <c r="V22" s="39"/>
+      <c r="W22" s="38"/>
+      <c r="X22" s="38"/>
+      <c r="Y22" s="39"/>
+      <c r="Z22" s="39"/>
+      <c r="AA22" s="39"/>
+      <c r="AB22" s="39"/>
+      <c r="AC22" s="39"/>
+      <c r="AD22" s="38"/>
+      <c r="AE22" s="39"/>
+      <c r="AF22" s="39"/>
+      <c r="AG22" s="39"/>
+      <c r="AH22" s="39"/>
+      <c r="AI22" s="39"/>
+      <c r="AJ22" s="38"/>
+      <c r="AK22" s="38"/>
+      <c r="AL22" s="40"/>
+      <c r="AM22" s="40"/>
+      <c r="AN22" s="40"/>
+      <c r="AO22" s="40"/>
+      <c r="AP22" s="40"/>
+      <c r="AQ22" s="41"/>
+      <c r="AR22" s="41"/>
+      <c r="AS22" s="39"/>
+      <c r="AT22" s="39"/>
+      <c r="AU22" s="39"/>
+      <c r="AV22" s="39"/>
+      <c r="AW22" s="39"/>
+      <c r="AX22" s="38"/>
+      <c r="AY22" s="38"/>
+      <c r="AZ22" s="39"/>
+      <c r="BA22" s="39"/>
+      <c r="BB22" s="39"/>
+      <c r="BC22" s="39"/>
+      <c r="BD22" s="39"/>
+      <c r="BE22" s="38"/>
+      <c r="BF22" s="38"/>
+      <c r="BG22" s="39"/>
+      <c r="BH22" s="39"/>
+      <c r="BI22" s="39"/>
+      <c r="BJ22" s="39"/>
+      <c r="BK22" s="39"/>
+      <c r="BL22" s="38"/>
+      <c r="BM22" s="38"/>
+      <c r="BN22" s="39"/>
+      <c r="BO22" s="39"/>
+      <c r="BP22" s="39"/>
+      <c r="BQ22" s="39"/>
+      <c r="BR22" s="39"/>
+      <c r="BS22" s="38"/>
+      <c r="BT22" s="38"/>
+      <c r="BU22" s="39"/>
+      <c r="BV22" s="39"/>
+      <c r="BW22" s="39"/>
+      <c r="BX22" s="39"/>
+      <c r="BY22" s="39"/>
+      <c r="BZ22" s="38"/>
+      <c r="CA22" s="38"/>
     </row>
-    <row r="23" spans="1:79" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40" t="s">
+    <row r="23" spans="1:79" x14ac:dyDescent="0.3">
+      <c r="A23" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="42"/>
-      <c r="T23" s="42"/>
-      <c r="U23" s="42"/>
-      <c r="V23" s="42"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="41"/>
-      <c r="Y23" s="42"/>
-      <c r="Z23" s="42"/>
-      <c r="AA23" s="42"/>
-      <c r="AB23" s="42"/>
-      <c r="AC23" s="42"/>
-      <c r="AD23" s="41"/>
-      <c r="AE23" s="42"/>
-      <c r="AF23" s="42"/>
-      <c r="AG23" s="42"/>
-      <c r="AH23" s="42"/>
-      <c r="AI23" s="42"/>
-      <c r="AJ23" s="41"/>
-      <c r="AK23" s="41"/>
-      <c r="AL23" s="44"/>
-      <c r="AM23" s="44"/>
-      <c r="AN23" s="44"/>
-      <c r="AO23" s="44"/>
-      <c r="AP23" s="44"/>
-      <c r="AQ23" s="45"/>
-      <c r="AR23" s="45"/>
-      <c r="AS23" s="42"/>
-      <c r="AT23" s="42"/>
-      <c r="AU23" s="42"/>
-      <c r="AV23" s="42"/>
-      <c r="AW23" s="42"/>
-      <c r="AX23" s="41"/>
-      <c r="AY23" s="41"/>
-      <c r="AZ23" s="42"/>
-      <c r="BA23" s="42"/>
-      <c r="BB23" s="42"/>
-      <c r="BC23" s="42"/>
-      <c r="BD23" s="42"/>
-      <c r="BE23" s="41"/>
-      <c r="BF23" s="41"/>
-      <c r="BG23" s="42"/>
-      <c r="BH23" s="42"/>
-      <c r="BI23" s="42"/>
-      <c r="BJ23" s="42"/>
-      <c r="BK23" s="42"/>
-      <c r="BL23" s="41"/>
-      <c r="BM23" s="41"/>
-      <c r="BN23" s="42"/>
-      <c r="BO23" s="42"/>
-      <c r="BP23" s="42"/>
-      <c r="BQ23" s="42"/>
-      <c r="BR23" s="42"/>
-      <c r="BS23" s="41"/>
-      <c r="BT23" s="41"/>
-      <c r="BU23" s="42"/>
-      <c r="BV23" s="42"/>
-      <c r="BW23" s="42"/>
-      <c r="BX23" s="42"/>
-      <c r="BY23" s="42"/>
-      <c r="BZ23" s="41"/>
-      <c r="CA23" s="41"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
+      <c r="V23" s="39"/>
+      <c r="W23" s="38"/>
+      <c r="X23" s="38"/>
+      <c r="Y23" s="39"/>
+      <c r="Z23" s="39"/>
+      <c r="AA23" s="39"/>
+      <c r="AB23" s="39"/>
+      <c r="AC23" s="39"/>
+      <c r="AD23" s="38"/>
+      <c r="AE23" s="39"/>
+      <c r="AF23" s="39"/>
+      <c r="AG23" s="39"/>
+      <c r="AH23" s="39"/>
+      <c r="AI23" s="39"/>
+      <c r="AJ23" s="38"/>
+      <c r="AK23" s="38"/>
+      <c r="AL23" s="40"/>
+      <c r="AM23" s="40"/>
+      <c r="AN23" s="40"/>
+      <c r="AO23" s="40"/>
+      <c r="AP23" s="40"/>
+      <c r="AQ23" s="41"/>
+      <c r="AR23" s="41"/>
+      <c r="AS23" s="39"/>
+      <c r="AT23" s="39"/>
+      <c r="AU23" s="39"/>
+      <c r="AV23" s="39"/>
+      <c r="AW23" s="39"/>
+      <c r="AX23" s="38"/>
+      <c r="AY23" s="38"/>
+      <c r="AZ23" s="39"/>
+      <c r="BA23" s="39"/>
+      <c r="BB23" s="39"/>
+      <c r="BC23" s="39"/>
+      <c r="BD23" s="39"/>
+      <c r="BE23" s="38"/>
+      <c r="BF23" s="38"/>
+      <c r="BG23" s="39"/>
+      <c r="BH23" s="39"/>
+      <c r="BI23" s="39"/>
+      <c r="BJ23" s="39"/>
+      <c r="BK23" s="39"/>
+      <c r="BL23" s="38"/>
+      <c r="BM23" s="38"/>
+      <c r="BN23" s="39"/>
+      <c r="BO23" s="39"/>
+      <c r="BP23" s="39"/>
+      <c r="BQ23" s="39"/>
+      <c r="BR23" s="39"/>
+      <c r="BS23" s="38"/>
+      <c r="BT23" s="38"/>
+      <c r="BU23" s="39"/>
+      <c r="BV23" s="39"/>
+      <c r="BW23" s="39"/>
+      <c r="BX23" s="39"/>
+      <c r="BY23" s="39"/>
+      <c r="BZ23" s="38"/>
+      <c r="CA23" s="38"/>
     </row>
     <row r="24" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
@@ -3172,13 +3174,13 @@
       <c r="AI24" s="32"/>
       <c r="AJ24" s="18"/>
       <c r="AK24" s="18"/>
-      <c r="AL24" s="44"/>
-      <c r="AM24" s="44"/>
-      <c r="AN24" s="44"/>
-      <c r="AO24" s="44"/>
-      <c r="AP24" s="44"/>
-      <c r="AQ24" s="45"/>
-      <c r="AR24" s="45"/>
+      <c r="AL24" s="40"/>
+      <c r="AM24" s="40"/>
+      <c r="AN24" s="40"/>
+      <c r="AO24" s="40"/>
+      <c r="AP24" s="40"/>
+      <c r="AQ24" s="41"/>
+      <c r="AR24" s="41"/>
       <c r="AS24" s="32"/>
       <c r="AT24" s="32"/>
       <c r="AU24" s="32"/>
@@ -3386,7 +3388,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="32"/>
@@ -3423,13 +3425,13 @@
       <c r="AI27" s="32"/>
       <c r="AJ27" s="18"/>
       <c r="AK27" s="18"/>
-      <c r="AL27" s="44"/>
-      <c r="AM27" s="44"/>
-      <c r="AN27" s="44"/>
-      <c r="AO27" s="44"/>
-      <c r="AP27" s="44"/>
-      <c r="AQ27" s="45"/>
-      <c r="AR27" s="45"/>
+      <c r="AL27" s="40"/>
+      <c r="AM27" s="40"/>
+      <c r="AN27" s="40"/>
+      <c r="AO27" s="40"/>
+      <c r="AP27" s="40"/>
+      <c r="AQ27" s="41"/>
+      <c r="AR27" s="41"/>
       <c r="AS27" s="32"/>
       <c r="AT27" s="32"/>
       <c r="AU27" s="32"/>
@@ -3471,7 +3473,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="32"/>
@@ -3556,7 +3558,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="32"/>
@@ -3641,7 +3643,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="32"/>
@@ -3692,20 +3694,20 @@
       <c r="AW30" s="32"/>
       <c r="AX30" s="18"/>
       <c r="AY30" s="18"/>
-      <c r="AZ30" s="44"/>
-      <c r="BA30" s="44"/>
-      <c r="BB30" s="44"/>
-      <c r="BC30" s="44"/>
-      <c r="BD30" s="44"/>
-      <c r="BE30" s="45"/>
-      <c r="BF30" s="45"/>
-      <c r="BG30" s="42"/>
-      <c r="BH30" s="42"/>
-      <c r="BI30" s="42"/>
-      <c r="BJ30" s="42"/>
-      <c r="BK30" s="42"/>
-      <c r="BL30" s="41"/>
-      <c r="BM30" s="41"/>
+      <c r="AZ30" s="40"/>
+      <c r="BA30" s="40"/>
+      <c r="BB30" s="40"/>
+      <c r="BC30" s="40"/>
+      <c r="BD30" s="40"/>
+      <c r="BE30" s="41"/>
+      <c r="BF30" s="41"/>
+      <c r="BG30" s="39"/>
+      <c r="BH30" s="39"/>
+      <c r="BI30" s="39"/>
+      <c r="BJ30" s="39"/>
+      <c r="BK30" s="39"/>
+      <c r="BL30" s="38"/>
+      <c r="BM30" s="38"/>
       <c r="BN30" s="32"/>
       <c r="BO30" s="32"/>
       <c r="BP30" s="32"/>
@@ -3867,13 +3869,13 @@
       <c r="BD32" s="32"/>
       <c r="BE32" s="18"/>
       <c r="BF32" s="18"/>
-      <c r="BG32" s="44"/>
-      <c r="BH32" s="44"/>
-      <c r="BI32" s="44"/>
-      <c r="BJ32" s="44"/>
-      <c r="BK32" s="44"/>
-      <c r="BL32" s="45"/>
-      <c r="BM32" s="45"/>
+      <c r="BG32" s="40"/>
+      <c r="BH32" s="40"/>
+      <c r="BI32" s="40"/>
+      <c r="BJ32" s="40"/>
+      <c r="BK32" s="40"/>
+      <c r="BL32" s="41"/>
+      <c r="BM32" s="41"/>
       <c r="BN32" s="36"/>
       <c r="BO32" s="36"/>
       <c r="BP32" s="36"/>

</xml_diff>

<commit_message>
organiser rdv et demande fourniture
</commit_message>
<xml_diff>
--- a/Documentations/Gant-JAVA-LPRS.xlsx
+++ b/Documentations/Gant-JAVA-LPRS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetLprs_Java\Documentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krimi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47605A2-79E4-4B19-8463-DAF7D030B53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DC81A6-5F80-4B5F-84C3-3DD9B8DB4B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0F548F66-3344-4CBB-911B-2A81E54675D2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="34">
   <si>
     <t>Site Lprs</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Krishmini</t>
+  </si>
+  <si>
+    <t>Sherazad</t>
+  </si>
+  <si>
+    <t>Sherazad, Krishmini</t>
   </si>
 </sst>
 </file>
@@ -875,14 +881,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57744C3F-6280-4959-BECA-99D079BDAE28}">
   <dimension ref="A1:CA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="77" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47.33203125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:79" ht="23.4" x14ac:dyDescent="0.45">
@@ -2120,9 +2126,7 @@
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
-      <c r="B12" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="B12" s="19"/>
       <c r="C12" s="17"/>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
@@ -2203,9 +2207,7 @@
     </row>
     <row r="13" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
-      <c r="B13" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="B13" s="19"/>
       <c r="C13" s="18"/>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
@@ -2372,7 +2374,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="32"/>
@@ -2624,9 +2626,7 @@
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="18"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
@@ -2707,9 +2707,7 @@
     </row>
     <row r="19" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="18"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
@@ -2876,7 +2874,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="32"/>
@@ -3046,7 +3044,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="38"/>
@@ -3131,7 +3129,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="32"/>
@@ -3213,9 +3211,7 @@
     </row>
     <row r="25" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
-      <c r="B25" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="B25" s="6"/>
       <c r="C25" s="18"/>
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
@@ -3382,7 +3378,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="32"/>
@@ -3467,7 +3463,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="32"/>
@@ -3552,7 +3548,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="32"/>
@@ -3637,7 +3633,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="32"/>

</xml_diff>